<commit_message>
HOMEACC-28: #comment Sumarize data/paypay/balance #time 3h 0m
</commit_message>
<xml_diff>
--- a/trial/MeoDemo_Final/Prepare_Manual/SpreadSheets/Manual_Balance.xlsx
+++ b/trial/MeoDemo_Final/Prepare_Manual/SpreadSheets/Manual_Balance.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minhphan/PycharmProjects/HomeAccounting/trial/MeoDemo_Final/Prepare_Manual/SpreadSheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A54E3F8-ABF3-5F45-A403-8C1FF59A79FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3C7490-B24C-2E40-A752-B5EB7E6153D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21080" yWindow="4140" windowWidth="28040" windowHeight="17440" xr2:uid="{211A79C5-B985-E94E-B0C1-2BF2BF8B9373}"/>
+    <workbookView xWindow="11600" yWindow="3100" windowWidth="28040" windowHeight="17440" xr2:uid="{211A79C5-B985-E94E-B0C1-2BF2BF8B9373}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$105</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$211</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="126">
   <si>
     <t>Date</t>
   </si>
@@ -303,6 +303,144 @@
   </si>
   <si>
     <t>Interest</t>
+  </si>
+  <si>
+    <t>Lopia</t>
+  </si>
+  <si>
+    <t>Clinic - Meo</t>
+  </si>
+  <si>
+    <t>Water Bill</t>
+  </si>
+  <si>
+    <t>Ring</t>
+  </si>
+  <si>
+    <t>VitCash</t>
+  </si>
+  <si>
+    <t>MacDonald</t>
+  </si>
+  <si>
+    <t>Gyomu Mark Nakamachidai</t>
+  </si>
+  <si>
+    <t>MeoYB</t>
+  </si>
+  <si>
+    <t>Vit won bet</t>
+  </si>
+  <si>
+    <t>Meo lost bet</t>
+  </si>
+  <si>
+    <t>Batting Center</t>
+  </si>
+  <si>
+    <t>Correct Muji Ball (wrong bill)</t>
+  </si>
+  <si>
+    <t>Seria</t>
+  </si>
+  <si>
+    <t>HomeCash</t>
+  </si>
+  <si>
+    <t>Kodomo No Kuni</t>
+  </si>
+  <si>
+    <t>Lunch at Kodomo Kuni</t>
+  </si>
+  <si>
+    <t>SIM</t>
+  </si>
+  <si>
+    <t>Mangoes</t>
+  </si>
+  <si>
+    <t>Meo loan</t>
+  </si>
+  <si>
+    <t>Sieu paid meal</t>
+  </si>
+  <si>
+    <t>Ramen</t>
+  </si>
+  <si>
+    <t>From Sieu</t>
+  </si>
+  <si>
+    <t>To Sieu</t>
+  </si>
+  <si>
+    <t>Print documents (claim)</t>
+  </si>
+  <si>
+    <t>Nancy stocks</t>
+  </si>
+  <si>
+    <t>Dish washing fee</t>
+  </si>
+  <si>
+    <t>Tool overdue fee</t>
+  </si>
+  <si>
+    <t>Overdue won</t>
+  </si>
+  <si>
+    <t>Shopping Kokoku</t>
+  </si>
+  <si>
+    <t>Akachan Honpo</t>
+  </si>
+  <si>
+    <t>HAC</t>
+  </si>
+  <si>
+    <t>Lalaport</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Electric, Gas</t>
+  </si>
+  <si>
+    <t>To Sieu (probably food/eating out)</t>
+  </si>
+  <si>
+    <t>Groceries</t>
+  </si>
+  <si>
+    <t>Eating Out</t>
+  </si>
+  <si>
+    <t>Charge from Credit Card</t>
+  </si>
+  <si>
+    <t>Credit Card marked as "Transfer"</t>
+  </si>
+  <si>
+    <t>Bonus</t>
+  </si>
+  <si>
+    <t>Bonus 2020/03</t>
+  </si>
+  <si>
+    <t>Bonus 2020/02</t>
+  </si>
+  <si>
+    <t>Bonus 2020/01</t>
+  </si>
+  <si>
+    <t>Need to add this category</t>
+  </si>
+  <si>
+    <t>Adjust to match latest balance</t>
+  </si>
+  <si>
+    <t>Money in Pocket now</t>
   </si>
 </sst>
 </file>
@@ -363,7 +501,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -394,6 +532,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -408,7 +552,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -456,6 +600,9 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -771,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C746422B-7B49-664B-A814-9E0769654701}">
-  <dimension ref="A1:O142"/>
+  <dimension ref="A1:O211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -785,7 +932,7 @@
     <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5" customWidth="1"/>
     <col min="6" max="7" width="16.1640625" customWidth="1"/>
-    <col min="8" max="8" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.5" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.5" style="3" bestFit="1" customWidth="1"/>
@@ -933,15 +1080,15 @@
         <v>6</v>
       </c>
       <c r="L5" s="3">
-        <f t="shared" ref="L5:L16" si="1">SUMIF(D:D,$K5,I:I)</f>
+        <f>SUMIF(D:D,$K5,I:I)</f>
         <v>50</v>
       </c>
       <c r="N5" t="s">
         <v>20</v>
       </c>
       <c r="O5" s="3">
-        <f>L5+L8+L13</f>
-        <v>11673002</v>
+        <f>L5+L8</f>
+        <v>11628402</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -975,15 +1122,15 @@
         <v>7</v>
       </c>
       <c r="L6" s="3">
-        <f t="shared" si="1"/>
+        <f>SUMIF(D:D,$K6,I:I)</f>
         <v>0</v>
       </c>
       <c r="N6" t="s">
         <v>21</v>
       </c>
       <c r="O6" s="3">
-        <f>L11+L15</f>
-        <v>11153644</v>
+        <f>L11+L15+L13</f>
+        <v>11198244</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -993,6 +1140,9 @@
       <c r="B7" t="s">
         <v>17</v>
       </c>
+      <c r="C7" s="3">
+        <v>56000</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1008,13 +1158,13 @@
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>56000</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>44</v>
       </c>
       <c r="L7" s="3">
-        <f t="shared" si="1"/>
+        <f>SUMIF(D:D,$K7,I:I)</f>
         <v>99656173</v>
       </c>
       <c r="N7" t="s">
@@ -1057,16 +1207,20 @@
         <v>8</v>
       </c>
       <c r="L8" s="3">
-        <f t="shared" si="1"/>
+        <f>SUMIF(D:D,$K8,I:I)</f>
         <v>11628352</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>44196</v>
+        <v>44287</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
+      </c>
+      <c r="C9" s="3">
+        <f>8259+2923</f>
+        <v>11182</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>12</v>
@@ -1079,17 +1233,17 @@
         <v>52</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>124</v>
       </c>
       <c r="I9">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>IF(G9="Out",C9*-1,C9)</f>
+        <v>11182</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="L9" s="3">
-        <f t="shared" si="1"/>
+        <f>SUMIF(D:D,$K9,I:I)</f>
         <v>16700</v>
       </c>
     </row>
@@ -1124,16 +1278,19 @@
         <v>10</v>
       </c>
       <c r="L10" s="3">
-        <f t="shared" si="1"/>
-        <v>178000</v>
+        <f>SUMIF(D:D,$K10,I:I)</f>
+        <v>146124</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>44196</v>
+        <v>43922</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
+      </c>
+      <c r="C11" s="3">
+        <v>8700</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>14</v>
@@ -1146,18 +1303,18 @@
         <v>52</v>
       </c>
       <c r="H11" t="s">
-        <v>18</v>
+        <v>125</v>
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8700</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L11" s="3">
-        <f t="shared" si="1"/>
-        <v>10540482</v>
+        <f>SUMIF(D:D,$K11,I:I)</f>
+        <v>10554742</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -1191,8 +1348,8 @@
         <v>12</v>
       </c>
       <c r="L12" s="3">
-        <f t="shared" si="1"/>
-        <v>3600</v>
+        <f>SUMIF(D:D,$K12,I:I)</f>
+        <v>2923</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -1202,6 +1359,9 @@
       <c r="B13" t="s">
         <v>17</v>
       </c>
+      <c r="C13" s="3">
+        <v>1000</v>
+      </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1217,14 +1377,14 @@
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="L13" s="16">
-        <f t="shared" si="1"/>
-        <v>44600</v>
+        <f>SUMIF(D:D,$K13,I:I)</f>
+        <v>6750</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -1255,8 +1415,8 @@
         <v>14</v>
       </c>
       <c r="L14" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>SUMIF(D:D,$K14,I:I)</f>
+        <v>8700</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
@@ -1287,8 +1447,8 @@
         <v>15</v>
       </c>
       <c r="L15" s="3">
-        <f t="shared" si="1"/>
-        <v>613162</v>
+        <f>SUMIF(D:D,$K15,I:I)</f>
+        <v>636752</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -1322,8 +1482,8 @@
         <v>16</v>
       </c>
       <c r="L16" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>SUMIF(D:D,$K16,I:I)</f>
+        <v>571</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -1410,7 +1570,7 @@
       </c>
       <c r="K19" s="5">
         <f>12070158-O5</f>
-        <v>397156</v>
+        <v>441756</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -2856,7 +3016,7 @@
         <v>53</v>
       </c>
       <c r="I81">
-        <f t="shared" ref="I81:I82" si="2">IF(G81="Out",C81*-1,C81)</f>
+        <f t="shared" ref="I81:I82" si="1">IF(G81="Out",C81*-1,C81)</f>
         <v>-15697</v>
       </c>
     </row>
@@ -2877,7 +3037,7 @@
         <v>52</v>
       </c>
       <c r="I82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>15697</v>
       </c>
     </row>
@@ -2922,7 +3082,7 @@
         <v>52</v>
       </c>
       <c r="I84">
-        <f t="shared" ref="I84:I85" si="3">IF(G84="Out",C84*-1,C84)</f>
+        <f t="shared" ref="I84:I85" si="2">IF(G84="Out",C84*-1,C84)</f>
         <v>107</v>
       </c>
     </row>
@@ -2946,7 +3106,7 @@
         <v>53</v>
       </c>
       <c r="I85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-107</v>
       </c>
     </row>
@@ -3093,7 +3253,7 @@
         <v>52</v>
       </c>
       <c r="I92">
-        <f t="shared" ref="I92:I123" si="4">IF(G92="Out",C92*-1,C92)</f>
+        <f t="shared" ref="I92:I123" si="3">IF(G92="Out",C92*-1,C92)</f>
         <v>218389</v>
       </c>
     </row>
@@ -3115,7 +3275,7 @@
         <v>52</v>
       </c>
       <c r="I93">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>10000</v>
       </c>
     </row>
@@ -3137,7 +3297,7 @@
         <v>53</v>
       </c>
       <c r="I94">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-10000</v>
       </c>
     </row>
@@ -3158,7 +3318,7 @@
         <v>52</v>
       </c>
       <c r="I95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2000</v>
       </c>
     </row>
@@ -3179,7 +3339,7 @@
         <v>53</v>
       </c>
       <c r="I96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-2000</v>
       </c>
     </row>
@@ -3200,7 +3360,7 @@
         <v>53</v>
       </c>
       <c r="I97">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-200000</v>
       </c>
     </row>
@@ -3221,7 +3381,7 @@
         <v>52</v>
       </c>
       <c r="I98">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>200000</v>
       </c>
     </row>
@@ -3242,7 +3402,7 @@
         <v>53</v>
       </c>
       <c r="I99">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-3600</v>
       </c>
     </row>
@@ -3263,7 +3423,7 @@
         <v>52</v>
       </c>
       <c r="I100">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3600</v>
       </c>
     </row>
@@ -3286,7 +3446,7 @@
         <v>53</v>
       </c>
       <c r="I101">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-2000</v>
       </c>
     </row>
@@ -3311,7 +3471,7 @@
         <v>53</v>
       </c>
       <c r="I102">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-24000</v>
       </c>
     </row>
@@ -3336,7 +3496,7 @@
         <v>52</v>
       </c>
       <c r="I103">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>24000</v>
       </c>
     </row>
@@ -3359,7 +3519,7 @@
         <v>53</v>
       </c>
       <c r="I104">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-20000</v>
       </c>
     </row>
@@ -3382,7 +3542,7 @@
         <v>52</v>
       </c>
       <c r="I105">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>20000</v>
       </c>
     </row>
@@ -3404,7 +3564,7 @@
         <v>53</v>
       </c>
       <c r="I106">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-5000</v>
       </c>
     </row>
@@ -3426,7 +3586,7 @@
         <v>52</v>
       </c>
       <c r="I107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>768138</v>
       </c>
     </row>
@@ -3448,7 +3608,7 @@
         <v>53</v>
       </c>
       <c r="I108">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-121000</v>
       </c>
     </row>
@@ -3469,7 +3629,7 @@
         <v>53</v>
       </c>
       <c r="I109">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-77000</v>
       </c>
     </row>
@@ -3490,7 +3650,7 @@
         <v>53</v>
       </c>
       <c r="I110">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-11980</v>
       </c>
     </row>
@@ -3511,7 +3671,7 @@
         <v>53</v>
       </c>
       <c r="I111">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-3722</v>
       </c>
     </row>
@@ -3532,7 +3692,7 @@
         <v>53</v>
       </c>
       <c r="I112">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-727</v>
       </c>
     </row>
@@ -3553,7 +3713,7 @@
         <v>52</v>
       </c>
       <c r="I113">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>727</v>
       </c>
     </row>
@@ -3574,7 +3734,7 @@
         <v>53</v>
       </c>
       <c r="I114">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-727</v>
       </c>
     </row>
@@ -3595,7 +3755,7 @@
         <v>53</v>
       </c>
       <c r="I115">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-21184</v>
       </c>
     </row>
@@ -3616,7 +3776,7 @@
         <v>53</v>
       </c>
       <c r="I116">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-980</v>
       </c>
     </row>
@@ -3637,7 +3797,7 @@
         <v>53</v>
       </c>
       <c r="I117">
-        <f t="shared" ref="I117:I118" si="5">IF(G117="Out",C117*-1,C117)</f>
+        <f t="shared" ref="I117:I118" si="4">IF(G117="Out",C117*-1,C117)</f>
         <v>-6956</v>
       </c>
     </row>
@@ -3658,7 +3818,7 @@
         <v>52</v>
       </c>
       <c r="I118">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6956</v>
       </c>
     </row>
@@ -3700,7 +3860,7 @@
         <v>53</v>
       </c>
       <c r="I120">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-106604</v>
       </c>
     </row>
@@ -3721,7 +3881,7 @@
         <v>53</v>
       </c>
       <c r="I121">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3742,7 +3902,7 @@
         <v>53</v>
       </c>
       <c r="I122">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-1518</v>
       </c>
     </row>
@@ -3763,7 +3923,7 @@
         <v>52</v>
       </c>
       <c r="I123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1518</v>
       </c>
     </row>
@@ -3828,7 +3988,7 @@
         <v>53</v>
       </c>
       <c r="I126">
-        <f t="shared" ref="I126:I140" si="6">IF(G126="Out",C126*-1,C126)</f>
+        <f t="shared" ref="I126:I140" si="5">IF(G126="Out",C126*-1,C126)</f>
         <v>-10000</v>
       </c>
     </row>
@@ -3849,7 +4009,7 @@
         <v>53</v>
       </c>
       <c r="I127">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-24200</v>
       </c>
     </row>
@@ -3873,11 +4033,11 @@
         <v>52</v>
       </c>
       <c r="I128">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>107</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
         <v>44261</v>
       </c>
@@ -3897,11 +4057,11 @@
         <v>53</v>
       </c>
       <c r="I129">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-107</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
         <v>44270</v>
       </c>
@@ -3918,11 +4078,11 @@
         <v>52</v>
       </c>
       <c r="I130">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>165260</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
         <v>44280</v>
       </c>
@@ -3939,11 +4099,11 @@
         <v>52</v>
       </c>
       <c r="I131">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1500</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
         <v>44286</v>
       </c>
@@ -3960,11 +4120,11 @@
         <v>53</v>
       </c>
       <c r="I132">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-397156</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
         <v>44286</v>
       </c>
@@ -3981,11 +4141,11 @@
         <v>52</v>
       </c>
       <c r="I133">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>397156</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
         <v>44270</v>
       </c>
@@ -4004,11 +4164,11 @@
         <v>53</v>
       </c>
       <c r="I134">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-2000</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
         <v>44262</v>
       </c>
@@ -4029,11 +4189,11 @@
         <v>53</v>
       </c>
       <c r="I135">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-30000</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
         <v>44262</v>
       </c>
@@ -4054,11 +4214,11 @@
         <v>52</v>
       </c>
       <c r="I136">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>30000</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
         <v>44285</v>
       </c>
@@ -4079,11 +4239,11 @@
         <v>53</v>
       </c>
       <c r="I137">
-        <f t="shared" ref="I137:I138" si="7">IF(G137="Out",C137*-1,C137)</f>
+        <f t="shared" ref="I137:I138" si="6">IF(G137="Out",C137*-1,C137)</f>
         <v>-74000</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
         <v>44285</v>
       </c>
@@ -4104,11 +4264,11 @@
         <v>52</v>
       </c>
       <c r="I138">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>74000</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A139" s="2">
         <v>44286</v>
       </c>
@@ -4127,11 +4287,11 @@
         <v>53</v>
       </c>
       <c r="I139">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-20000</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
         <v>44286</v>
       </c>
@@ -4150,11 +4310,11 @@
         <v>52</v>
       </c>
       <c r="I140">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>20000</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A141" s="2">
         <v>44287</v>
       </c>
@@ -4171,11 +4331,11 @@
         <v>52</v>
       </c>
       <c r="I141">
-        <f t="shared" ref="I141" si="8">IF(G141="Out",C141*-1,C141)</f>
+        <f t="shared" ref="I141:I204" si="7">IF(G141="Out",C141*-1,C141)</f>
         <v>50</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
         <v>44287</v>
       </c>
@@ -4192,12 +4352,1541 @@
         <v>52</v>
       </c>
       <c r="I142">
-        <f t="shared" ref="I142" si="9">IF(G142="Out",C142*-1,C142)</f>
+        <f t="shared" si="7"/>
         <v>42</v>
       </c>
     </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A143" s="2">
+        <v>44198</v>
+      </c>
+      <c r="B143" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C143" s="3">
+        <v>2771</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G143" t="s">
+        <v>53</v>
+      </c>
+      <c r="I143">
+        <f t="shared" si="7"/>
+        <v>-2771</v>
+      </c>
+      <c r="K143" s="3"/>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A144" s="2">
+        <v>44202</v>
+      </c>
+      <c r="B144" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C144" s="3">
+        <v>2190</v>
+      </c>
+      <c r="D144" t="s">
+        <v>93</v>
+      </c>
+      <c r="G144" t="s">
+        <v>53</v>
+      </c>
+      <c r="I144">
+        <f t="shared" si="7"/>
+        <v>-2190</v>
+      </c>
+      <c r="K144" s="3"/>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A145" s="35">
+        <v>44206</v>
+      </c>
+      <c r="B145" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="C145" s="37">
+        <v>4761</v>
+      </c>
+      <c r="D145" t="s">
+        <v>93</v>
+      </c>
+      <c r="G145" t="s">
+        <v>53</v>
+      </c>
+      <c r="I145">
+        <f t="shared" si="7"/>
+        <v>-4761</v>
+      </c>
+      <c r="K145" s="37"/>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A146" s="35">
+        <v>44212</v>
+      </c>
+      <c r="B146" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="C146" s="37">
+        <v>6401</v>
+      </c>
+      <c r="D146" t="s">
+        <v>93</v>
+      </c>
+      <c r="G146" t="s">
+        <v>53</v>
+      </c>
+      <c r="I146">
+        <f t="shared" si="7"/>
+        <v>-6401</v>
+      </c>
+      <c r="K146" s="37"/>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A147" s="35">
+        <v>44215</v>
+      </c>
+      <c r="B147" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="C147" s="37">
+        <v>2728</v>
+      </c>
+      <c r="D147" t="s">
+        <v>93</v>
+      </c>
+      <c r="G147" t="s">
+        <v>53</v>
+      </c>
+      <c r="I147">
+        <f t="shared" si="7"/>
+        <v>-2728</v>
+      </c>
+      <c r="K147" s="37"/>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A148" s="2">
+        <v>44222</v>
+      </c>
+      <c r="B148" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="C148" s="3">
+        <v>4615</v>
+      </c>
+      <c r="D148" t="s">
+        <v>93</v>
+      </c>
+      <c r="G148" t="s">
+        <v>53</v>
+      </c>
+      <c r="I148">
+        <f t="shared" si="7"/>
+        <v>-4615</v>
+      </c>
+      <c r="K148" s="3"/>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A149" s="2">
+        <v>44223</v>
+      </c>
+      <c r="B149" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C149" s="3">
+        <v>3875</v>
+      </c>
+      <c r="D149" t="s">
+        <v>93</v>
+      </c>
+      <c r="G149" t="s">
+        <v>53</v>
+      </c>
+      <c r="I149">
+        <f t="shared" si="7"/>
+        <v>-3875</v>
+      </c>
+      <c r="K149" s="3"/>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A150" s="2">
+        <v>44231</v>
+      </c>
+      <c r="B150" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C150" s="3">
+        <v>2276</v>
+      </c>
+      <c r="D150" t="s">
+        <v>93</v>
+      </c>
+      <c r="G150" t="s">
+        <v>53</v>
+      </c>
+      <c r="I150">
+        <f t="shared" si="7"/>
+        <v>-2276</v>
+      </c>
+      <c r="K150" s="3"/>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A151" s="2">
+        <v>44231</v>
+      </c>
+      <c r="B151" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C151" s="3">
+        <v>429</v>
+      </c>
+      <c r="D151" t="s">
+        <v>84</v>
+      </c>
+      <c r="G151" t="s">
+        <v>53</v>
+      </c>
+      <c r="I151">
+        <f t="shared" si="7"/>
+        <v>-429</v>
+      </c>
+      <c r="K151" s="3"/>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A152" s="2">
+        <v>44238</v>
+      </c>
+      <c r="B152" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="C152" s="17">
+        <v>800</v>
+      </c>
+      <c r="D152" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G152" t="s">
+        <v>53</v>
+      </c>
+      <c r="I152">
+        <f t="shared" si="7"/>
+        <v>-800</v>
+      </c>
+      <c r="K152" s="17"/>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A153" s="2">
+        <v>44243</v>
+      </c>
+      <c r="B153" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C153" s="3">
+        <v>5753</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G153" t="s">
+        <v>53</v>
+      </c>
+      <c r="I153">
+        <f t="shared" si="7"/>
+        <v>-5753</v>
+      </c>
+      <c r="K153" s="3"/>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A154" s="2">
+        <v>44243</v>
+      </c>
+      <c r="B154" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C154" s="3">
+        <v>2379</v>
+      </c>
+      <c r="D154" t="s">
+        <v>93</v>
+      </c>
+      <c r="G154" t="s">
+        <v>53</v>
+      </c>
+      <c r="I154">
+        <f t="shared" si="7"/>
+        <v>-2379</v>
+      </c>
+      <c r="K154" s="3"/>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A155" s="2">
+        <v>44249</v>
+      </c>
+      <c r="B155" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C155" s="3">
+        <v>10000</v>
+      </c>
+      <c r="D155" t="s">
+        <v>87</v>
+      </c>
+      <c r="G155" t="s">
+        <v>53</v>
+      </c>
+      <c r="I155">
+        <f t="shared" si="7"/>
+        <v>-10000</v>
+      </c>
+      <c r="K155" s="3"/>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A156" s="2">
+        <v>44249</v>
+      </c>
+      <c r="B156" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C156" s="3">
+        <v>10000</v>
+      </c>
+      <c r="D156" t="s">
+        <v>69</v>
+      </c>
+      <c r="G156" t="s">
+        <v>52</v>
+      </c>
+      <c r="I156">
+        <f t="shared" si="7"/>
+        <v>10000</v>
+      </c>
+      <c r="K156" s="3"/>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A157" s="2">
+        <v>44250</v>
+      </c>
+      <c r="B157" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C157" s="3">
+        <v>2409</v>
+      </c>
+      <c r="D157" t="s">
+        <v>93</v>
+      </c>
+      <c r="G157" t="s">
+        <v>53</v>
+      </c>
+      <c r="I157">
+        <f t="shared" si="7"/>
+        <v>-2409</v>
+      </c>
+      <c r="K157" s="3"/>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A158" s="2">
+        <v>44250</v>
+      </c>
+      <c r="B158" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="C158" s="3">
+        <v>1000</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G158" t="s">
+        <v>53</v>
+      </c>
+      <c r="I158">
+        <f t="shared" si="7"/>
+        <v>-1000</v>
+      </c>
+      <c r="K158" s="3"/>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A159" s="2">
+        <v>44250</v>
+      </c>
+      <c r="B159" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="C159" s="3">
+        <v>1000</v>
+      </c>
+      <c r="D159" t="s">
+        <v>87</v>
+      </c>
+      <c r="G159" t="s">
+        <v>53</v>
+      </c>
+      <c r="I159">
+        <f t="shared" si="7"/>
+        <v>-1000</v>
+      </c>
+      <c r="K159" s="3"/>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A160" s="2">
+        <v>44250</v>
+      </c>
+      <c r="B160" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="C160" s="3">
+        <v>1000</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G160" t="s">
+        <v>52</v>
+      </c>
+      <c r="I160">
+        <f t="shared" si="7"/>
+        <v>1000</v>
+      </c>
+      <c r="K160" s="3"/>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A161" s="2">
+        <v>44250</v>
+      </c>
+      <c r="B161" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="C161" s="3">
+        <v>590</v>
+      </c>
+      <c r="D161" t="s">
+        <v>87</v>
+      </c>
+      <c r="G161" t="s">
+        <v>53</v>
+      </c>
+      <c r="I161">
+        <f t="shared" si="7"/>
+        <v>-590</v>
+      </c>
+      <c r="K161" s="3"/>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A162" s="2">
+        <v>44250</v>
+      </c>
+      <c r="B162" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="C162" s="3">
+        <v>590</v>
+      </c>
+      <c r="D162" t="s">
+        <v>69</v>
+      </c>
+      <c r="G162" t="s">
+        <v>52</v>
+      </c>
+      <c r="I162">
+        <f t="shared" si="7"/>
+        <v>590</v>
+      </c>
+      <c r="K162" s="3"/>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A163" s="2">
+        <v>44253</v>
+      </c>
+      <c r="B163" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="C163" s="3">
+        <v>660</v>
+      </c>
+      <c r="D163" t="s">
+        <v>93</v>
+      </c>
+      <c r="G163" t="s">
+        <v>53</v>
+      </c>
+      <c r="I163">
+        <f t="shared" si="7"/>
+        <v>-660</v>
+      </c>
+      <c r="K163" s="3"/>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A164" s="2">
+        <v>44253</v>
+      </c>
+      <c r="B164" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C164" s="3">
+        <v>3268</v>
+      </c>
+      <c r="D164" t="s">
+        <v>93</v>
+      </c>
+      <c r="G164" t="s">
+        <v>53</v>
+      </c>
+      <c r="I164">
+        <f t="shared" si="7"/>
+        <v>-3268</v>
+      </c>
+      <c r="K164" s="3"/>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A165" s="2">
+        <v>44254</v>
+      </c>
+      <c r="B165" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C165" s="3">
+        <v>1200</v>
+      </c>
+      <c r="D165" t="s">
+        <v>93</v>
+      </c>
+      <c r="G165" t="s">
+        <v>53</v>
+      </c>
+      <c r="I165">
+        <f t="shared" si="7"/>
+        <v>-1200</v>
+      </c>
+      <c r="K165" s="3"/>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A166" s="2">
+        <v>44254</v>
+      </c>
+      <c r="B166" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="C166" s="3">
+        <v>2210</v>
+      </c>
+      <c r="D166" t="s">
+        <v>93</v>
+      </c>
+      <c r="G166" t="s">
+        <v>53</v>
+      </c>
+      <c r="I166">
+        <f t="shared" si="7"/>
+        <v>-2210</v>
+      </c>
+      <c r="K166" s="3"/>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A167" s="2">
+        <v>44256</v>
+      </c>
+      <c r="B167" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C167" s="3">
+        <v>1500</v>
+      </c>
+      <c r="D167" t="s">
+        <v>75</v>
+      </c>
+      <c r="G167" t="s">
+        <v>52</v>
+      </c>
+      <c r="I167">
+        <f t="shared" si="7"/>
+        <v>1500</v>
+      </c>
+      <c r="K167" s="3"/>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A168" s="2">
+        <v>44256</v>
+      </c>
+      <c r="B168" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C168" s="3">
+        <v>2400</v>
+      </c>
+      <c r="D168" t="s">
+        <v>75</v>
+      </c>
+      <c r="G168" t="s">
+        <v>53</v>
+      </c>
+      <c r="I168">
+        <f t="shared" si="7"/>
+        <v>-2400</v>
+      </c>
+      <c r="K168" s="3"/>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A169" s="2">
+        <v>44256</v>
+      </c>
+      <c r="B169" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C169" s="3">
+        <v>2400</v>
+      </c>
+      <c r="D169" t="s">
+        <v>87</v>
+      </c>
+      <c r="G169" t="s">
+        <v>53</v>
+      </c>
+      <c r="I169">
+        <f t="shared" si="7"/>
+        <v>-2400</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A170" s="2">
+        <v>44256</v>
+      </c>
+      <c r="B170" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C170" s="3">
+        <v>2400</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G170" t="s">
+        <v>52</v>
+      </c>
+      <c r="I170">
+        <f t="shared" si="7"/>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A171" s="2">
+        <v>44257</v>
+      </c>
+      <c r="B171" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C171" s="3">
+        <v>6955</v>
+      </c>
+      <c r="D171" t="s">
+        <v>93</v>
+      </c>
+      <c r="G171" t="s">
+        <v>53</v>
+      </c>
+      <c r="I171">
+        <f t="shared" si="7"/>
+        <v>-6955</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A172" s="2">
+        <v>44261</v>
+      </c>
+      <c r="B172" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C172" s="3">
+        <v>1100</v>
+      </c>
+      <c r="D172" t="s">
+        <v>87</v>
+      </c>
+      <c r="G172" t="s">
+        <v>53</v>
+      </c>
+      <c r="I172">
+        <f t="shared" si="7"/>
+        <v>-1100</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A173" s="2">
+        <v>44261</v>
+      </c>
+      <c r="B173" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C173" s="3">
+        <v>1100</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G173" t="s">
+        <v>52</v>
+      </c>
+      <c r="I173">
+        <f t="shared" si="7"/>
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A174" s="2">
+        <v>44261</v>
+      </c>
+      <c r="B174" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C174" s="3">
+        <v>1100</v>
+      </c>
+      <c r="D174" t="s">
+        <v>93</v>
+      </c>
+      <c r="G174" t="s">
+        <v>53</v>
+      </c>
+      <c r="I174">
+        <f t="shared" si="7"/>
+        <v>-1100</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A175" s="2">
+        <v>44261</v>
+      </c>
+      <c r="B175" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C175" s="3">
+        <v>9550</v>
+      </c>
+      <c r="D175" t="s">
+        <v>93</v>
+      </c>
+      <c r="G175" t="s">
+        <v>53</v>
+      </c>
+      <c r="I175">
+        <f t="shared" si="7"/>
+        <v>-9550</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A176" s="2">
+        <v>44264</v>
+      </c>
+      <c r="B176" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C176" s="3">
+        <v>3522</v>
+      </c>
+      <c r="D176" t="s">
+        <v>93</v>
+      </c>
+      <c r="G176" t="s">
+        <v>53</v>
+      </c>
+      <c r="I176">
+        <f t="shared" si="7"/>
+        <v>-3522</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A177" s="2">
+        <v>44263</v>
+      </c>
+      <c r="B177" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C177" s="3">
+        <v>2303</v>
+      </c>
+      <c r="D177" t="s">
+        <v>93</v>
+      </c>
+      <c r="G177" t="s">
+        <v>53</v>
+      </c>
+      <c r="I177">
+        <f t="shared" si="7"/>
+        <v>-2303</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A178" s="2">
+        <v>44269</v>
+      </c>
+      <c r="B178" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="C178" s="3">
+        <v>2410</v>
+      </c>
+      <c r="D178" t="s">
+        <v>75</v>
+      </c>
+      <c r="G178" t="s">
+        <v>52</v>
+      </c>
+      <c r="I178">
+        <f t="shared" si="7"/>
+        <v>2410</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A179" s="2">
+        <v>44266</v>
+      </c>
+      <c r="B179" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C179" s="3">
+        <v>2925</v>
+      </c>
+      <c r="D179" t="s">
+        <v>93</v>
+      </c>
+      <c r="G179" t="s">
+        <v>53</v>
+      </c>
+      <c r="I179">
+        <f t="shared" si="7"/>
+        <v>-2925</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A180" s="2">
+        <v>44269</v>
+      </c>
+      <c r="B180" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C180" s="3">
+        <v>2530</v>
+      </c>
+      <c r="D180" t="s">
+        <v>93</v>
+      </c>
+      <c r="G180" t="s">
+        <v>53</v>
+      </c>
+      <c r="I180">
+        <f t="shared" si="7"/>
+        <v>-2530</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A181" s="2">
+        <v>44269</v>
+      </c>
+      <c r="B181" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="C181" s="3">
+        <v>1480</v>
+      </c>
+      <c r="D181" t="s">
+        <v>75</v>
+      </c>
+      <c r="G181" t="s">
+        <v>53</v>
+      </c>
+      <c r="I181">
+        <f t="shared" si="7"/>
+        <v>-1480</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A182" s="2">
+        <v>44269</v>
+      </c>
+      <c r="B182" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C182" s="3">
+        <v>3098</v>
+      </c>
+      <c r="D182" t="s">
+        <v>93</v>
+      </c>
+      <c r="G182" t="s">
+        <v>53</v>
+      </c>
+      <c r="I182">
+        <f t="shared" si="7"/>
+        <v>-3098</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A183" s="2">
+        <v>44275</v>
+      </c>
+      <c r="B183" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C183" s="3">
+        <v>4280</v>
+      </c>
+      <c r="D183" t="s">
+        <v>93</v>
+      </c>
+      <c r="G183" t="s">
+        <v>53</v>
+      </c>
+      <c r="I183">
+        <f t="shared" si="7"/>
+        <v>-4280</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A184" s="2">
+        <v>44278</v>
+      </c>
+      <c r="B184" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="C184" s="3">
+        <v>240</v>
+      </c>
+      <c r="D184" t="s">
+        <v>87</v>
+      </c>
+      <c r="G184" t="s">
+        <v>52</v>
+      </c>
+      <c r="I184">
+        <f t="shared" si="7"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A185" s="2">
+        <v>44278</v>
+      </c>
+      <c r="B185" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="C185" s="3">
+        <v>240</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G185" t="s">
+        <v>53</v>
+      </c>
+      <c r="I185">
+        <f t="shared" si="7"/>
+        <v>-240</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A186" s="2">
+        <v>44278</v>
+      </c>
+      <c r="B186" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="C186" s="3">
+        <v>319</v>
+      </c>
+      <c r="D186" t="s">
+        <v>93</v>
+      </c>
+      <c r="G186" t="s">
+        <v>53</v>
+      </c>
+      <c r="I186">
+        <f t="shared" si="7"/>
+        <v>-319</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A187" s="2">
+        <v>44283</v>
+      </c>
+      <c r="B187" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="C187" s="3">
+        <v>3000</v>
+      </c>
+      <c r="D187" t="s">
+        <v>87</v>
+      </c>
+      <c r="G187" t="s">
+        <v>53</v>
+      </c>
+      <c r="I187">
+        <f t="shared" si="7"/>
+        <v>-3000</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A188" s="2">
+        <v>44283</v>
+      </c>
+      <c r="B188" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="C188" s="3">
+        <v>3000</v>
+      </c>
+      <c r="D188" t="s">
+        <v>69</v>
+      </c>
+      <c r="G188" t="s">
+        <v>52</v>
+      </c>
+      <c r="I188">
+        <f t="shared" si="7"/>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A189" s="2">
+        <v>44284</v>
+      </c>
+      <c r="B189" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C189" s="3">
+        <v>2798</v>
+      </c>
+      <c r="D189" t="s">
+        <v>93</v>
+      </c>
+      <c r="G189" t="s">
+        <v>53</v>
+      </c>
+      <c r="I189">
+        <f t="shared" si="7"/>
+        <v>-2798</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A190" s="2">
+        <v>44287</v>
+      </c>
+      <c r="B190" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="C190" s="3">
+        <v>20000</v>
+      </c>
+      <c r="D190" t="s">
+        <v>87</v>
+      </c>
+      <c r="G190" t="s">
+        <v>53</v>
+      </c>
+      <c r="I190">
+        <f t="shared" si="7"/>
+        <v>-20000</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A191" s="2">
+        <v>44287</v>
+      </c>
+      <c r="B191" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="C191" s="3">
+        <v>10000</v>
+      </c>
+      <c r="D191" t="s">
+        <v>69</v>
+      </c>
+      <c r="G191" t="s">
+        <v>52</v>
+      </c>
+      <c r="I191">
+        <f t="shared" si="7"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A192" s="2">
+        <v>44287</v>
+      </c>
+      <c r="B192" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="C192" s="3">
+        <v>10000</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G192" t="s">
+        <v>52</v>
+      </c>
+      <c r="I192">
+        <f t="shared" si="7"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A193" s="2">
+        <v>44198</v>
+      </c>
+      <c r="B193" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="C193" s="3">
+        <v>2602</v>
+      </c>
+      <c r="D193" t="s">
+        <v>75</v>
+      </c>
+      <c r="G193" t="s">
+        <v>53</v>
+      </c>
+      <c r="I193">
+        <f t="shared" si="7"/>
+        <v>-2602</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A194" s="2">
+        <v>44198</v>
+      </c>
+      <c r="B194" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="C194" s="3">
+        <v>158</v>
+      </c>
+      <c r="D194" t="s">
+        <v>75</v>
+      </c>
+      <c r="G194" t="s">
+        <v>53</v>
+      </c>
+      <c r="I194">
+        <f t="shared" si="7"/>
+        <v>-158</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A195" s="2">
+        <v>44198</v>
+      </c>
+      <c r="B195" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="C195" s="3">
+        <v>2048</v>
+      </c>
+      <c r="D195" t="s">
+        <v>75</v>
+      </c>
+      <c r="G195" t="s">
+        <v>53</v>
+      </c>
+      <c r="I195">
+        <f t="shared" si="7"/>
+        <v>-2048</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A196" s="2">
+        <v>44199</v>
+      </c>
+      <c r="B196" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="C196" s="3">
+        <v>1650</v>
+      </c>
+      <c r="D196" t="s">
+        <v>75</v>
+      </c>
+      <c r="E196" t="s">
+        <v>112</v>
+      </c>
+      <c r="G196" t="s">
+        <v>53</v>
+      </c>
+      <c r="I196">
+        <f t="shared" si="7"/>
+        <v>-1650</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A197" s="2">
+        <v>44226</v>
+      </c>
+      <c r="B197" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="C197" s="3">
+        <v>12793</v>
+      </c>
+      <c r="D197" t="s">
+        <v>75</v>
+      </c>
+      <c r="G197" t="s">
+        <v>53</v>
+      </c>
+      <c r="I197">
+        <f t="shared" si="7"/>
+        <v>-12793</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A198" s="2">
+        <v>44256</v>
+      </c>
+      <c r="B198" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="C198" s="3">
+        <v>11533</v>
+      </c>
+      <c r="D198" t="s">
+        <v>75</v>
+      </c>
+      <c r="G198" t="s">
+        <v>53</v>
+      </c>
+      <c r="I198">
+        <f t="shared" si="7"/>
+        <v>-11533</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A199" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B199" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="C199" s="3">
+        <v>2500</v>
+      </c>
+      <c r="D199" t="s">
+        <v>75</v>
+      </c>
+      <c r="E199" t="s">
+        <v>115</v>
+      </c>
+      <c r="G199" t="s">
+        <v>53</v>
+      </c>
+      <c r="I199">
+        <f t="shared" si="7"/>
+        <v>-2500</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A200" s="2">
+        <v>44244</v>
+      </c>
+      <c r="B200" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="C200" s="3">
+        <v>1270</v>
+      </c>
+      <c r="D200" t="s">
+        <v>75</v>
+      </c>
+      <c r="E200" t="s">
+        <v>116</v>
+      </c>
+      <c r="G200" t="s">
+        <v>53</v>
+      </c>
+      <c r="I200">
+        <f t="shared" si="7"/>
+        <v>-1270</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A201" s="2">
+        <v>44256</v>
+      </c>
+      <c r="B201" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="C201" s="3">
+        <v>900</v>
+      </c>
+      <c r="D201" t="s">
+        <v>75</v>
+      </c>
+      <c r="E201" t="s">
+        <v>115</v>
+      </c>
+      <c r="G201" t="s">
+        <v>53</v>
+      </c>
+      <c r="I201">
+        <f t="shared" si="7"/>
+        <v>-900</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A202" s="2">
+        <v>44270</v>
+      </c>
+      <c r="B202" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="C202" s="3">
+        <v>900</v>
+      </c>
+      <c r="D202" t="s">
+        <v>75</v>
+      </c>
+      <c r="E202" t="s">
+        <v>115</v>
+      </c>
+      <c r="G202" t="s">
+        <v>53</v>
+      </c>
+      <c r="I202">
+        <f t="shared" si="7"/>
+        <v>-900</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A203" s="2">
+        <v>44226</v>
+      </c>
+      <c r="B203" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="C203" s="3">
+        <v>6408</v>
+      </c>
+      <c r="D203" t="s">
+        <v>75</v>
+      </c>
+      <c r="E203" t="s">
+        <v>54</v>
+      </c>
+      <c r="G203" t="s">
+        <v>52</v>
+      </c>
+      <c r="H203" t="s">
+        <v>118</v>
+      </c>
+      <c r="I203">
+        <f t="shared" si="7"/>
+        <v>6408</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A204" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B204" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C204" s="3">
+        <v>200</v>
+      </c>
+      <c r="D204" t="s">
+        <v>75</v>
+      </c>
+      <c r="E204" t="s">
+        <v>46</v>
+      </c>
+      <c r="G204" t="s">
+        <v>52</v>
+      </c>
+      <c r="I204">
+        <f t="shared" si="7"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A205" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B205" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C205" s="3">
+        <v>2400</v>
+      </c>
+      <c r="D205" t="s">
+        <v>75</v>
+      </c>
+      <c r="E205" t="s">
+        <v>46</v>
+      </c>
+      <c r="G205" t="s">
+        <v>52</v>
+      </c>
+      <c r="I205">
+        <f t="shared" ref="I205:I211" si="8">IF(G205="Out",C205*-1,C205)</f>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A206" s="2">
+        <v>44214</v>
+      </c>
+      <c r="B206" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C206" s="3">
+        <v>1500</v>
+      </c>
+      <c r="D206" t="s">
+        <v>75</v>
+      </c>
+      <c r="E206" t="s">
+        <v>46</v>
+      </c>
+      <c r="G206" t="s">
+        <v>52</v>
+      </c>
+      <c r="I206">
+        <f t="shared" si="8"/>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A207" s="2">
+        <v>44227</v>
+      </c>
+      <c r="B207" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C207" s="3">
+        <v>5600</v>
+      </c>
+      <c r="D207" t="s">
+        <v>75</v>
+      </c>
+      <c r="E207" t="s">
+        <v>46</v>
+      </c>
+      <c r="G207" t="s">
+        <v>52</v>
+      </c>
+      <c r="I207">
+        <f t="shared" si="8"/>
+        <v>5600</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A208" s="2">
+        <v>44229</v>
+      </c>
+      <c r="B208" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C208" s="3">
+        <v>3060</v>
+      </c>
+      <c r="D208" t="s">
+        <v>75</v>
+      </c>
+      <c r="E208" t="s">
+        <v>46</v>
+      </c>
+      <c r="G208" t="s">
+        <v>52</v>
+      </c>
+      <c r="I208">
+        <f t="shared" si="8"/>
+        <v>3060</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A209" s="2">
+        <v>44286</v>
+      </c>
+      <c r="B209" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C209" s="3">
+        <v>3123</v>
+      </c>
+      <c r="D209" t="s">
+        <v>75</v>
+      </c>
+      <c r="E209" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="G209" t="s">
+        <v>52</v>
+      </c>
+      <c r="H209" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="I209">
+        <f t="shared" si="8"/>
+        <v>3123</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A210" s="2">
+        <v>44255</v>
+      </c>
+      <c r="B210" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C210" s="3">
+        <v>2013</v>
+      </c>
+      <c r="D210" t="s">
+        <v>75</v>
+      </c>
+      <c r="E210" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="G210" t="s">
+        <v>52</v>
+      </c>
+      <c r="H210" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="I210">
+        <f t="shared" si="8"/>
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A211" s="2">
+        <v>44227</v>
+      </c>
+      <c r="B211" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="C211" s="3">
+        <v>961</v>
+      </c>
+      <c r="D211" t="s">
+        <v>75</v>
+      </c>
+      <c r="E211" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="G211" t="s">
+        <v>52</v>
+      </c>
+      <c r="H211" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="I211">
+        <f t="shared" si="8"/>
+        <v>961</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:P105" xr:uid="{528EF4BF-5565-314F-90E0-92999827C614}"/>
+  <autoFilter ref="A1:P211" xr:uid="{528EF4BF-5565-314F-90E0-92999827C614}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
HOMEACC-28: #time 1h 30m Import 2020/02 Data
</commit_message>
<xml_diff>
--- a/trial/MeoDemo_Final/Prepare_Manual/SpreadSheets/Manual_Balance.xlsx
+++ b/trial/MeoDemo_Final/Prepare_Manual/SpreadSheets/Manual_Balance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minhphan/PycharmProjects/HomeAccounting/trial/MeoDemo_Final/Prepare_Manual/SpreadSheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029DDB20-082F-C34E-BE9B-C20F77668CE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F007297-4245-4541-9648-E80FF91A0FF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19360" yWindow="8540" windowWidth="28040" windowHeight="17440" xr2:uid="{211A79C5-B985-E94E-B0C1-2BF2BF8B9373}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="141">
   <si>
     <t>Date</t>
   </si>
@@ -479,6 +479,12 @@
   </si>
   <si>
     <t>Medical</t>
+  </si>
+  <si>
+    <t>Uniqlo</t>
+  </si>
+  <si>
+    <t>Fashion</t>
   </si>
 </sst>
 </file>
@@ -890,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C746422B-7B49-664B-A814-9E0769654701}">
-  <dimension ref="A1:O219"/>
+  <dimension ref="A1:O221"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A188" workbookViewId="0">
+      <selection activeCell="E218" sqref="E218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1303,7 +1309,7 @@
       </c>
       <c r="L11" s="2">
         <f t="shared" si="1"/>
-        <v>10564742</v>
+        <v>10566161</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -1446,7 +1452,7 @@
       </c>
       <c r="L15" s="2">
         <f t="shared" si="1"/>
-        <v>626752</v>
+        <v>625333</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -6210,7 +6216,7 @@
         <v>50</v>
       </c>
       <c r="I205" s="7">
-        <f t="shared" ref="I205:I219" si="9">IF(G205="Out",C205*-1,C205)</f>
+        <f t="shared" ref="I205:I221" si="9">IF(G205="Out",C205*-1,C205)</f>
         <v>2400</v>
       </c>
     </row>
@@ -6477,7 +6483,7 @@
         <v>84</v>
       </c>
       <c r="E216" s="7" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="G216" s="7" t="s">
         <v>51</v>
@@ -6501,7 +6507,7 @@
         <v>84</v>
       </c>
       <c r="E217" s="7" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="G217" s="7" t="s">
         <v>51</v>
@@ -6525,7 +6531,7 @@
         <v>84</v>
       </c>
       <c r="E218" s="7" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="G218" s="7" t="s">
         <v>51</v>
@@ -6557,6 +6563,54 @@
       <c r="I219" s="7">
         <f t="shared" si="9"/>
         <v>-32842</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A220" s="11">
+        <v>44212</v>
+      </c>
+      <c r="B220" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C220" s="12">
+        <v>1419</v>
+      </c>
+      <c r="D220" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="E220" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G220" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I220" s="7">
+        <f t="shared" si="9"/>
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A221" s="11">
+        <v>44212</v>
+      </c>
+      <c r="B221" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C221" s="12">
+        <v>1419</v>
+      </c>
+      <c r="D221" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E221" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="G221" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I221" s="7">
+        <f t="shared" si="9"/>
+        <v>-1419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HOMEACC-28: #time 0h 5m Update Vit's transactions
</commit_message>
<xml_diff>
--- a/trial/MeoDemo_Final/Prepare_Manual/SpreadSheets/Manual_Balance.xlsx
+++ b/trial/MeoDemo_Final/Prepare_Manual/SpreadSheets/Manual_Balance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minhphan/PycharmProjects/HomeAccounting/trial/MeoDemo_Final/Prepare_Manual/SpreadSheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F007297-4245-4541-9648-E80FF91A0FF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A162B8C8-F014-2344-B4B7-A32B3DFFEDB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19360" yWindow="8540" windowWidth="28040" windowHeight="17440" xr2:uid="{211A79C5-B985-E94E-B0C1-2BF2BF8B9373}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="142">
   <si>
     <t>Date</t>
   </si>
@@ -485,6 +485,9 @@
   </si>
   <si>
     <t>Fashion</t>
+  </si>
+  <si>
+    <t>Tamaplaza Terrace shopping</t>
   </si>
 </sst>
 </file>
@@ -896,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C746422B-7B49-664B-A814-9E0769654701}">
-  <dimension ref="A1:O221"/>
+  <dimension ref="A1:O225"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A188" workbookViewId="0">
-      <selection activeCell="E218" sqref="E218"/>
+      <selection activeCell="C226" sqref="C226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1309,7 +1312,7 @@
       </c>
       <c r="L11" s="2">
         <f t="shared" si="1"/>
-        <v>10566161</v>
+        <v>10578833</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -1452,7 +1455,7 @@
       </c>
       <c r="L15" s="2">
         <f t="shared" si="1"/>
-        <v>625333</v>
+        <v>612661</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -6611,6 +6614,102 @@
       <c r="I221" s="7">
         <f t="shared" si="9"/>
         <v>-1419</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A222" s="11">
+        <v>44179</v>
+      </c>
+      <c r="B222" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C222" s="12">
+        <v>11055</v>
+      </c>
+      <c r="D222" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="E222" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G222" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I222" s="7">
+        <f t="shared" ref="I222:I225" si="10">IF(G222="Out",C222*-1,C222)</f>
+        <v>11055</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A223" s="11">
+        <v>44179</v>
+      </c>
+      <c r="B223" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C223" s="12">
+        <v>11055</v>
+      </c>
+      <c r="D223" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E223" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="G223" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I223" s="7">
+        <f t="shared" si="10"/>
+        <v>-11055</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A224" s="11">
+        <v>44184</v>
+      </c>
+      <c r="B224" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C224" s="12">
+        <v>1617</v>
+      </c>
+      <c r="D224" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="E224" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G224" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I224" s="7">
+        <f t="shared" si="10"/>
+        <v>1617</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A225" s="11">
+        <v>44184</v>
+      </c>
+      <c r="B225" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C225" s="12">
+        <v>1617</v>
+      </c>
+      <c r="D225" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E225" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="G225" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I225" s="7">
+        <f t="shared" si="10"/>
+        <v>-1617</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HOMEACC-28: #time 0h 15m Update Vit's transactions
</commit_message>
<xml_diff>
--- a/trial/MeoDemo_Final/Prepare_Manual/SpreadSheets/Manual_Balance.xlsx
+++ b/trial/MeoDemo_Final/Prepare_Manual/SpreadSheets/Manual_Balance.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minhphan/PycharmProjects/HomeAccounting/trial/MeoDemo_Final/Prepare_Manual/SpreadSheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A162B8C8-F014-2344-B4B7-A32B3DFFEDB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BAC50E-B0E9-0343-A129-E6482A334391}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19360" yWindow="8540" windowWidth="28040" windowHeight="17440" xr2:uid="{211A79C5-B985-E94E-B0C1-2BF2BF8B9373}"/>
+    <workbookView xWindow="7240" yWindow="1860" windowWidth="28040" windowHeight="17440" xr2:uid="{211A79C5-B985-E94E-B0C1-2BF2BF8B9373}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$219</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$225</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -901,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C746422B-7B49-664B-A814-9E0769654701}">
   <dimension ref="A1:O225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A188" workbookViewId="0">
-      <selection activeCell="C226" sqref="C226"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6713,7 +6713,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P219" xr:uid="{528EF4BF-5565-314F-90E0-92999827C614}"/>
+  <autoFilter ref="A1:P225" xr:uid="{528EF4BF-5565-314F-90E0-92999827C614}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>